<commit_message>
Javascriptexcel: Veritabanı ve excel arası kontroller kaldırıldı.
</commit_message>
<xml_diff>
--- a/javascriptexcel/excel.xlsx
+++ b/javascriptexcel/excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="121">
   <si>
     <t>tckn</t>
   </si>
@@ -22,64 +22,361 @@
     <t>isim-soyisim</t>
   </si>
   <si>
-    <t>Rol</t>
-  </si>
-  <si>
-    <t>sicil no</t>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>sicilno</t>
   </si>
   <si>
     <t>kartid</t>
   </si>
   <si>
-    <t>12345678902</t>
-  </si>
-  <si>
-    <t>Ahmet Mehmet</t>
+    <t>Mustafa Ekşi</t>
+  </si>
+  <si>
+    <t>Yazılımcı</t>
+  </si>
+  <si>
+    <t>2Yz1T1</t>
+  </si>
+  <si>
+    <t>0548066</t>
+  </si>
+  <si>
+    <t>Deneme 1</t>
   </si>
   <si>
     <t>Yardımcı</t>
   </si>
   <si>
-    <t>2Yr1T1</t>
-  </si>
-  <si>
-    <t>0543839</t>
-  </si>
-  <si>
-    <t>12345678903</t>
-  </si>
-  <si>
-    <t>Şeyda Gündüz</t>
-  </si>
-  <si>
-    <t>Yazılımcı</t>
-  </si>
-  <si>
-    <t>2Yz1T2</t>
-  </si>
-  <si>
-    <t>0576480</t>
-  </si>
-  <si>
-    <t>12345678901</t>
-  </si>
-  <si>
-    <t>Mustafa Ekşi</t>
+    <t>2Yr1T2</t>
+  </si>
+  <si>
+    <t>0557556</t>
+  </si>
+  <si>
+    <t>Deneme 2</t>
   </si>
   <si>
     <t>2Yz2T3</t>
   </si>
   <si>
-    <t>0540902</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>2Yr2T4</t>
-  </si>
-  <si>
-    <t>0598221</t>
+    <t>0596809</t>
+  </si>
+  <si>
+    <t>Deneme 3</t>
+  </si>
+  <si>
+    <t>2Yz3T4</t>
+  </si>
+  <si>
+    <t>0556206</t>
+  </si>
+  <si>
+    <t>Deneme 4</t>
+  </si>
+  <si>
+    <t>2Yr2T5</t>
+  </si>
+  <si>
+    <t>0534946</t>
+  </si>
+  <si>
+    <t>Deneme 5</t>
+  </si>
+  <si>
+    <t>2Yr3T6</t>
+  </si>
+  <si>
+    <t>0575856</t>
+  </si>
+  <si>
+    <t>Deneme 6</t>
+  </si>
+  <si>
+    <t>2Yz4T7</t>
+  </si>
+  <si>
+    <t>0589524</t>
+  </si>
+  <si>
+    <t>Deneme 7</t>
+  </si>
+  <si>
+    <t>2Yz5T8</t>
+  </si>
+  <si>
+    <t>0505252</t>
+  </si>
+  <si>
+    <t>Deneme 8</t>
+  </si>
+  <si>
+    <t>2Yr4T9</t>
+  </si>
+  <si>
+    <t>0503722</t>
+  </si>
+  <si>
+    <t>Deneme 9</t>
+  </si>
+  <si>
+    <t>2Yr5T10</t>
+  </si>
+  <si>
+    <t>0585283</t>
+  </si>
+  <si>
+    <t>Deneme 10</t>
+  </si>
+  <si>
+    <t>2Yz6T11</t>
+  </si>
+  <si>
+    <t>0543388</t>
+  </si>
+  <si>
+    <t>Deneme 11</t>
+  </si>
+  <si>
+    <t>2Yz7T12</t>
+  </si>
+  <si>
+    <t>0531971</t>
+  </si>
+  <si>
+    <t>Deneme 12</t>
+  </si>
+  <si>
+    <t>2Yr6T13</t>
+  </si>
+  <si>
+    <t>0535025</t>
+  </si>
+  <si>
+    <t>Deneme 13</t>
+  </si>
+  <si>
+    <t>2Yr7T14</t>
+  </si>
+  <si>
+    <t>0549107</t>
+  </si>
+  <si>
+    <t>Deneme 14</t>
+  </si>
+  <si>
+    <t>2Yz8T15</t>
+  </si>
+  <si>
+    <t>0559375</t>
+  </si>
+  <si>
+    <t>Deneme 15</t>
+  </si>
+  <si>
+    <t>2Yz9T16</t>
+  </si>
+  <si>
+    <t>0542635</t>
+  </si>
+  <si>
+    <t>Deneme 16</t>
+  </si>
+  <si>
+    <t>2Yr8T17</t>
+  </si>
+  <si>
+    <t>0515728</t>
+  </si>
+  <si>
+    <t>Deneme 17</t>
+  </si>
+  <si>
+    <t>2Yr9T18</t>
+  </si>
+  <si>
+    <t>0513127</t>
+  </si>
+  <si>
+    <t>Deneme 18</t>
+  </si>
+  <si>
+    <t>2Yz10T19</t>
+  </si>
+  <si>
+    <t>0594059</t>
+  </si>
+  <si>
+    <t>Deneme 19</t>
+  </si>
+  <si>
+    <t>2Yr10T20</t>
+  </si>
+  <si>
+    <t>0541061</t>
+  </si>
+  <si>
+    <t>Deneme 20</t>
+  </si>
+  <si>
+    <t>2Yz11T21</t>
+  </si>
+  <si>
+    <t>0574807</t>
+  </si>
+  <si>
+    <t>Deneme 21</t>
+  </si>
+  <si>
+    <t>2Yz12T22</t>
+  </si>
+  <si>
+    <t>0562062</t>
+  </si>
+  <si>
+    <t>Deneme 22</t>
+  </si>
+  <si>
+    <t>2Yr11T23</t>
+  </si>
+  <si>
+    <t>0522161</t>
+  </si>
+  <si>
+    <t>Deneme 23</t>
+  </si>
+  <si>
+    <t>2Yr12T24</t>
+  </si>
+  <si>
+    <t>0526731</t>
+  </si>
+  <si>
+    <t>Deneme 24</t>
+  </si>
+  <si>
+    <t>2Yz13T25</t>
+  </si>
+  <si>
+    <t>0505452</t>
+  </si>
+  <si>
+    <t>Deneme 25</t>
+  </si>
+  <si>
+    <t>2Yz14T26</t>
+  </si>
+  <si>
+    <t>0551502</t>
+  </si>
+  <si>
+    <t>Deneme 26</t>
+  </si>
+  <si>
+    <t>2Yr13T27</t>
+  </si>
+  <si>
+    <t>0525991</t>
+  </si>
+  <si>
+    <t>Deneme 27</t>
+  </si>
+  <si>
+    <t>2Yr14T28</t>
+  </si>
+  <si>
+    <t>0504945</t>
+  </si>
+  <si>
+    <t>Deneme 28</t>
+  </si>
+  <si>
+    <t>2Yz15T29</t>
+  </si>
+  <si>
+    <t>0588009</t>
+  </si>
+  <si>
+    <t>Deneme 29</t>
+  </si>
+  <si>
+    <t>2Yz16T30</t>
+  </si>
+  <si>
+    <t>0588368</t>
+  </si>
+  <si>
+    <t>Deneme 30</t>
+  </si>
+  <si>
+    <t>2Yr15T31</t>
+  </si>
+  <si>
+    <t>0559022</t>
+  </si>
+  <si>
+    <t>Deneme 31</t>
+  </si>
+  <si>
+    <t>2Yz17T32</t>
+  </si>
+  <si>
+    <t>0529434</t>
+  </si>
+  <si>
+    <t>Deneme 32</t>
+  </si>
+  <si>
+    <t>2Yz18T33</t>
+  </si>
+  <si>
+    <t>0567724</t>
+  </si>
+  <si>
+    <t>Deneme 33</t>
+  </si>
+  <si>
+    <t>2Yr16T34</t>
+  </si>
+  <si>
+    <t>0526462</t>
+  </si>
+  <si>
+    <t>Deneme 34</t>
+  </si>
+  <si>
+    <t>2Yr17T35</t>
+  </si>
+  <si>
+    <t>0596146</t>
+  </si>
+  <si>
+    <t>Deneme 35</t>
+  </si>
+  <si>
+    <t>2Yz19T36</t>
+  </si>
+  <si>
+    <t>0596264</t>
+  </si>
+  <si>
+    <t>Deneme 36</t>
+  </si>
+  <si>
+    <t>2Yz20T37</t>
+  </si>
+  <si>
+    <t>0503940</t>
+  </si>
+  <si>
+    <t>Deneme 37</t>
+  </si>
+  <si>
+    <t>2Yr18T38</t>
+  </si>
+  <si>
+    <t>0514139</t>
   </si>
 </sst>
 </file>
@@ -121,9 +418,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +931,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,9 +939,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.00390625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.00390625" customWidth="1"/>
-    <col min="4" max="4" width="15.8515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,77 +957,871 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>12345678900</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>12345678901</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>12345678902</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>12345678903</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>12345678904</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>12345678905</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>12345678906</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>12345678907</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12345678908</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>12345678909</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>12345678910</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12345678911</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12345678912</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>12345678913</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>12345678914</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>12345678915</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>12345678916</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>12345678917</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>12345678918</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>12345678919</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>12345678920</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>12345678921</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>12345678922</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>12345678923</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>12345678924</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>12345678925</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>12345678926</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>12345678927</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>12345678928</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>12345678929</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>12345678930</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>12345678931</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>12345678932</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>12345678933</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>12345678934</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>12345678935</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>12345678936</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>12345678937</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>12345678904</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>12345678905</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>12345678906</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>12345678907</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>12345678908</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>12345678909</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>12345678910</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>12345678911</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>12345678912</v>
+      </c>
+      <c r="B48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>12345678913</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>12345678914</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>12345678915</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>12345678916</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>12345678917</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>12345678918</v>
+      </c>
+      <c r="B54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>12345678919</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>12345678920</v>
+      </c>
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" ht="14.25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>12345678921</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7007874015748032" right="0.7007874015748032" top="0.7519685039370079" bottom="0.7519685039370079" header="0.3" footer="0.3"/>

</xml_diff>